<commit_message>
enable maxRepeatLength configurable in rule file
</commit_message>
<xml_diff>
--- a/conf/rush_rules.xlsx
+++ b/conf/rush_rules.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">#this list is optimized for shorter rule length rules for semeval were added</t>
   </si>
   <si>
-    <t xml:space="preserve">#FastCRules.maxRepeatLength = 100;</t>
+    <t xml:space="preserve">@maxRepeatLength</t>
   </si>
   <si>
     <t xml:space="preserve">#stbegin is the marker for sentence begin, the span of sentence will start at the begin of the captured group</t>
@@ -2599,6 +2599,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2682,16 +2683,16 @@
   </sheetPr>
   <dimension ref="A1:C951"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A547" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A526" activeCellId="0" sqref="A526:C951"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="177.163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.62755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.47959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.48469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2777,6 +2778,9 @@
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>14</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>